<commit_message>
browser stack plan updated
</commit_message>
<xml_diff>
--- a/OrangeHRMWebApplication/artifact/data/OHRM_01_signup.data.xlsx
+++ b/OrangeHRMWebApplication/artifact/data/OHRM_01_signup.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -79,31 +79,16 @@
     <t>browserstack</t>
   </si>
   <si>
-    <t>nexial.browserstack.browser</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>nexial.browserstack.username</t>
   </si>
   <si>
     <t>sandhiyamunisamy1</t>
   </si>
   <si>
-    <t>nexial.browserstack.automateKey</t>
+    <t>nexial.browserstack.automatekey</t>
   </si>
   <si>
     <t>rNG6nSGKb3vEz5bJ5pqW</t>
-  </si>
-  <si>
-    <t>browserstack.local</t>
-  </si>
-  <si>
-    <t>nexial.browserstack.reportStatus</t>
-  </si>
-  <si>
-    <t>execution</t>
   </si>
   <si>
     <t>url</t>
@@ -900,11 +885,12 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.249946592608417"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.14996795556505"/>
+          <bgColor theme="4" tint="0.599963377788629"/>
         </patternFill>
       </fill>
     </dxf>
@@ -924,25 +910,12 @@
       <font>
         <b val="1"/>
         <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.249946592608417"/>
+        <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.599963377788629"/>
+          <bgColor theme="0" tint="-0.14996795556505"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
       </fill>
     </dxf>
     <dxf>
@@ -957,6 +930,18 @@
         <patternFill patternType="solid">
           <bgColor theme="0" tint="-0.0499893185216834"/>
         </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
       </fill>
     </dxf>
   </dxfs>
@@ -1240,10 +1225,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AAA207"/>
+  <dimension ref="A1:AAA204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A9" sqref="$A9:$XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1359,7 +1344,7 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="HA11" s="8"/>
@@ -1370,93 +1355,66 @@
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="HA12" s="8"/>
       <c r="AAA12" s="9"/>
     </row>
     <row r="13" ht="23" customHeight="1" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="HA13" s="8"/>
       <c r="AAA13" s="9"/>
     </row>
     <row r="14" ht="23" customHeight="1" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="4" t="s">
         <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="HA14" s="8"/>
       <c r="AAA14" s="9"/>
     </row>
-    <row r="15" ht="23" customHeight="1" spans="1:703">
+    <row r="15" ht="23" customHeight="1" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="HA15" s="8"/>
-      <c r="AAA15" s="9"/>
-    </row>
-    <row r="16" ht="23" customHeight="1" spans="1:703">
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" ht="23" customHeight="1" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="HA16" s="8"/>
-      <c r="AAA16" s="9"/>
-    </row>
-    <row r="17" ht="23" customHeight="1" spans="1:703">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" ht="23" customHeight="1" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="HA17" s="8"/>
-      <c r="AAA17" s="9"/>
+        <v>31</v>
+      </c>
     </row>
     <row r="18" ht="23" customHeight="1" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" ht="23" customHeight="1" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" ht="23" customHeight="1" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" ht="23" customHeight="1" spans="1:2">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="5">
+      <c r="B18" s="5">
         <v>7502987295</v>
       </c>
     </row>
+    <row r="19" ht="23" customHeight="1"/>
+    <row r="20" ht="23" customHeight="1"/>
+    <row r="21" ht="23" customHeight="1"/>
     <row r="22" ht="23" customHeight="1"/>
     <row r="23" ht="23" customHeight="1"/>
     <row r="24" ht="23" customHeight="1"/>
@@ -1640,71 +1598,49 @@
     <row r="202" ht="23" customHeight="1"/>
     <row r="203" ht="23" customHeight="1"/>
     <row r="204" ht="23" customHeight="1"/>
-    <row r="205" ht="23" customHeight="1"/>
-    <row r="206" ht="23" customHeight="1"/>
-    <row r="207" ht="23" customHeight="1"/>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
+  <conditionalFormatting sqref="A1:A10">
+    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A12,LEN("nexial."))="nexial."</formula>
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A12,LEN("nexial.scope."))="nexial.scope."</formula>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="5">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
+  <conditionalFormatting sqref="A11:A1048576">
+    <cfRule type="beginsWith" dxfId="0" priority="16" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A11,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A11,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="18" stopIfTrue="1">
+      <formula>LEN(TRIM(A11))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B10">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="sentry.scope."</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A1048576">
-    <cfRule type="beginsWith" dxfId="2" priority="11" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A14,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="12" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A14,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="13" stopIfTrue="1">
-      <formula>LEN(TRIM(A14))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A11 A13">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="7" stopIfTrue="1" operator="equal" text="nexial.">
-      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="6" stopIfTrue="1" operator="equal" text="nexial.scope.">
-      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B11 B13">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="10">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="B11:B12 B19:B1048576">
+    <cfRule type="expression" dxfId="3" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="sentry.scope."</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22:B1048576 B14:B15">
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="15">
-      <formula>LEN(TRIM(B14))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
+      <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1" display="https://www.orangehrm.com/"/>
-    <hyperlink ref="B18" r:id="rId2" display="sandhiya.munisamy@atmecs.com"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://www.orangehrm.com/"/>
+    <hyperlink ref="B15" r:id="rId2" display="sandhiya.munisamy@atmecs.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>